<commit_message>
feat: add audio_url generate param
</commit_message>
<xml_diff>
--- a/static/file/batch_create_video_template.xlsx
+++ b/static/file/batch_create_video_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chen/Desktop/code/work/surreal-engine-playground/static/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEE2055-9F4F-EB44-8202-0B99139BD8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6490A3DF-65AB-F342-A856-E3BA4EF639D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35900" yWindow="-1460" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1280" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>pose_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,10 @@
   </si>
   <si>
     <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>audio_url</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,39 +475,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="27.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="24" customHeight="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:4" ht="24" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -511,7 +518,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F1:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="G1:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>